<commit_message>
more working through data to see how to resolve operational days
</commit_message>
<xml_diff>
--- a/Yalbac_Camera_Locations.xlsx
+++ b/Yalbac_Camera_Locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82392066-B010-0644-BBFD-465BA0CA43F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F632EB8-254F-A34C-8640-B71F6238B859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="2860" windowWidth="23260" windowHeight="12580" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11161,8 +11161,8 @@
   <dimension ref="A1:S80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11173,6 +11173,8 @@
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.83203125" style="62" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15202,8 +15204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>